<commit_message>
week3 day3 coding challenge
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>March 30 Friday</t>
+  </si>
+  <si>
+    <t>Lecture class in JS</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -327,6 +330,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -336,11 +341,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -677,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -782,8 +789,8 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
+      <c r="C14" t="s">
+        <v>81</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
@@ -814,6 +821,9 @@
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
@@ -1029,7 +1039,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B18" r:id="rId1" tooltip="Workshop: OO JavaScript Mini Challenges"/>
-    <hyperlink ref="C14" r:id="rId2" tooltip="Workshop: OO JavaScript Mini Challenges"/>
+    <hyperlink ref="C18" r:id="rId2" tooltip="Workshop: OO JavaScript Mini Challenges"/>
     <hyperlink ref="C26" r:id="rId3" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
     <hyperlink ref="D24" r:id="rId4" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
   </hyperlinks>

</xml_diff>

<commit_message>
week 4 day 4 sass
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -280,13 +280,16 @@
   </si>
   <si>
     <t>DB/heroku</t>
+  </si>
+  <si>
+    <t>Movie API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -315,6 +318,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -359,7 +367,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -374,8 +382,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -386,8 +407,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -396,6 +418,19 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -732,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -844,20 +879,20 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
         <v>25</v>
       </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="E16" t="s">
-        <v>27</v>
+      <c r="F16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -906,45 +941,50 @@
       <c r="E23" t="s">
         <v>35</v>
       </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="D24" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E24" t="s">
         <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="s">
-        <v>37</v>
+      <c r="D25" t="s">
+        <v>39</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="C26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E26" t="s">
-        <v>38</v>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -959,19 +999,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="2:6">
@@ -993,19 +1033,19 @@
     </row>
     <row r="36" spans="2:6">
       <c r="B36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" t="s">
         <v>85</v>
       </c>
+      <c r="E36" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -1023,17 +1063,6 @@
       </c>
       <c r="F39" s="7" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="44" spans="2:6">
@@ -1126,7 +1155,6 @@
     <hyperlink ref="B18" r:id="rId1" tooltip="Workshop: OO JavaScript Mini Challenges"/>
     <hyperlink ref="C18" r:id="rId2" tooltip="Workshop: OO JavaScript Mini Challenges"/>
     <hyperlink ref="C26" r:id="rId3" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
-    <hyperlink ref="D24" r:id="rId4" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
week 7 day 2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -283,13 +283,73 @@
   </si>
   <si>
     <t>Movie API</t>
+  </si>
+  <si>
+    <t>Rails Welcome</t>
+  </si>
+  <si>
+    <t>Devise</t>
+  </si>
+  <si>
+    <t>Paperclip</t>
+  </si>
+  <si>
+    <t>Partials</t>
+  </si>
+  <si>
+    <t>assets pipeline</t>
+  </si>
+  <si>
+    <t>Rails Blog</t>
+  </si>
+  <si>
+    <t>partials</t>
+  </si>
+  <si>
+    <t>many-to-many</t>
+  </si>
+  <si>
+    <t>Shipped</t>
+  </si>
+  <si>
+    <t>test driven develoment</t>
+  </si>
+  <si>
+    <t>api integration</t>
+  </si>
+  <si>
+    <t>Heroku</t>
+  </si>
+  <si>
+    <t>April 2 Monday</t>
+  </si>
+  <si>
+    <t>April 3 Tuesday</t>
+  </si>
+  <si>
+    <t>April 4 Wednesday</t>
+  </si>
+  <si>
+    <t>April 5 Thursday</t>
+  </si>
+  <si>
+    <t>Final group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final </t>
+  </si>
+  <si>
+    <t>database integrity</t>
+  </si>
+  <si>
+    <t>lambda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,8 +385,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +424,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -367,7 +458,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,8 +486,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -406,10 +507,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -431,6 +538,16 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -765,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -981,10 +1098,10 @@
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -1048,106 +1165,249 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
-      <c r="B39" s="5" t="s">
+    <row r="39" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B39" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="7" t="s">
+    <row r="40" spans="2:6">
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="D41" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="D43" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B44" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
-      <c r="B48" s="7" t="s">
+    <row r="45" spans="2:6">
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" s="13" customFormat="1">
+      <c r="C47" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B48" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
-      <c r="B52" t="s">
+    <row r="49" spans="2:6">
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B52" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
-      <c r="B56" t="s">
+    <row r="55" spans="2:6">
+      <c r="F55" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B56" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
-      <c r="B60" t="s">
+    <row r="59" spans="2:6" s="12" customFormat="1">
+      <c r="B59" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" s="9" customFormat="1" ht="18">
+      <c r="B60" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" s="9" customFormat="1" ht="18">
+      <c r="B65" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 9 is shaping
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>April 4 Wednesday</t>
-  </si>
-  <si>
-    <t>April 5 Thursday</t>
   </si>
   <si>
     <t>Final group</t>
@@ -896,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1254,12 +1251,12 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="2:6" s="13" customFormat="1">
@@ -1328,10 +1325,10 @@
     </row>
     <row r="55" spans="2:6">
       <c r="E55" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="2:6" s="9" customFormat="1" ht="18">
@@ -1353,19 +1350,19 @@
     </row>
     <row r="59" spans="2:6" s="12" customFormat="1">
       <c r="B59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="F59" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="60" spans="2:6" s="9" customFormat="1" ht="18">
@@ -1387,22 +1384,22 @@
     </row>
     <row r="64" spans="2:6">
       <c r="B64" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" s="9" customFormat="1" ht="18">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" s="9" customFormat="1" ht="18">
       <c r="B65" s="9" t="s">
         <v>100</v>
       </c>
@@ -1412,19 +1409,16 @@
       <c r="D65" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E65" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5">
+    </row>
+    <row r="68" spans="2:4">
       <c r="B68" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1434,7 +1428,6 @@
     <hyperlink ref="C26" r:id="rId3" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
week 10 day 1
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -312,12 +312,6 @@
     <t>Shipped</t>
   </si>
   <si>
-    <t>test driven develoment</t>
-  </si>
-  <si>
-    <t>api integration</t>
-  </si>
-  <si>
     <t>Heroku</t>
   </si>
   <si>
@@ -340,6 +334,18 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>April 5 Thursday</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>sick</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +451,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF660066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -455,7 +467,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -499,8 +511,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -518,8 +531,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -557,6 +571,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -893,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1213,7 +1228,7 @@
         <v>92</v>
       </c>
       <c r="F41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="2:6">
@@ -1251,12 +1266,12 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="2:6" s="13" customFormat="1">
@@ -1277,28 +1292,31 @@
       <c r="B48" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="C49" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>108</v>
+      </c>
+      <c r="F49" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -1307,10 +1325,10 @@
       </c>
     </row>
     <row r="52" spans="2:6" s="9" customFormat="1" ht="18">
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="15" t="s">
         <v>67</v>
       </c>
       <c r="D52" s="10" t="s">
@@ -1323,12 +1341,20 @@
         <v>70</v>
       </c>
     </row>
+    <row r="53" spans="2:6">
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="55" spans="2:6">
       <c r="E55" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="2:6" s="9" customFormat="1" ht="18">
@@ -1350,19 +1376,19 @@
     </row>
     <row r="59" spans="2:6" s="12" customFormat="1">
       <c r="B59" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="2:6" s="9" customFormat="1" ht="18">
@@ -1384,41 +1410,47 @@
     </row>
     <row r="64" spans="2:6">
       <c r="B64" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" s="9" customFormat="1" ht="18">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" s="9" customFormat="1" ht="18">
       <c r="B65" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D65" s="9" t="s">
+      <c r="E65" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="68" spans="2:4">
-      <c r="B68" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="C68" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1428,6 +1460,7 @@
     <hyperlink ref="C26" r:id="rId3" tooltip="Workshop: OO JavaScript Mini Challenges" display="OO JavaScript Mini Challenges"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
day 2 and three week one updated
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jan. 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="April 2018" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="211">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -346,13 +347,319 @@
   </si>
   <si>
     <t>sick</t>
+  </si>
+  <si>
+    <t>April 16 - Monday</t>
+  </si>
+  <si>
+    <t>April 17 - Tuesday</t>
+  </si>
+  <si>
+    <t>April 18 - Wednesday</t>
+  </si>
+  <si>
+    <t>April 19 - Thursday</t>
+  </si>
+  <si>
+    <t>April 20 - Friday</t>
+  </si>
+  <si>
+    <t>April 23 - Monday</t>
+  </si>
+  <si>
+    <t>April 24 - Tuesday</t>
+  </si>
+  <si>
+    <t>April 25 - Wednesday</t>
+  </si>
+  <si>
+    <t>April 26 - Thursday</t>
+  </si>
+  <si>
+    <t>April 27 - Friday</t>
+  </si>
+  <si>
+    <t>April 30 - Monday</t>
+  </si>
+  <si>
+    <t>May 1 - Tuesday</t>
+  </si>
+  <si>
+    <t>May 2 - Wedensday</t>
+  </si>
+  <si>
+    <t>May 3 - Thursday</t>
+  </si>
+  <si>
+    <t>May 4 - Friday</t>
+  </si>
+  <si>
+    <t>May 7 - Monday</t>
+  </si>
+  <si>
+    <t>May 8 - Tuesday</t>
+  </si>
+  <si>
+    <t>May 9 - Wednesday</t>
+  </si>
+  <si>
+    <t>May 10 - Thursday</t>
+  </si>
+  <si>
+    <t>May 11 - Friday</t>
+  </si>
+  <si>
+    <t>May 14 - Monday</t>
+  </si>
+  <si>
+    <t>May 15 - Tuesday</t>
+  </si>
+  <si>
+    <t>May 16 - Wednesday</t>
+  </si>
+  <si>
+    <t>May 17 - Thursday</t>
+  </si>
+  <si>
+    <t>May 18 - Friday</t>
+  </si>
+  <si>
+    <t>May 21 - Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 22 - Tuesday </t>
+  </si>
+  <si>
+    <t>May 23 - Wednesday</t>
+  </si>
+  <si>
+    <t>May 24 - Thursday</t>
+  </si>
+  <si>
+    <t>May 25 - Friday</t>
+  </si>
+  <si>
+    <t>May 28 - Monday</t>
+  </si>
+  <si>
+    <t>May 29 - Tuesday</t>
+  </si>
+  <si>
+    <t>May 30 - Wednesday</t>
+  </si>
+  <si>
+    <t>May 31 - Thursday</t>
+  </si>
+  <si>
+    <t>June 1 - Friday</t>
+  </si>
+  <si>
+    <t>June 4 Monday</t>
+  </si>
+  <si>
+    <t>June 5 - Tuesday</t>
+  </si>
+  <si>
+    <t>June 6 - Wednesday</t>
+  </si>
+  <si>
+    <t>June 7 - Thursday</t>
+  </si>
+  <si>
+    <t>June 8 - Friday</t>
+  </si>
+  <si>
+    <t>June 11 - Monday</t>
+  </si>
+  <si>
+    <t>June 12 - Tuesday</t>
+  </si>
+  <si>
+    <t>June 13 - Wednesday</t>
+  </si>
+  <si>
+    <t>June 14 - Thursday</t>
+  </si>
+  <si>
+    <t>June 15 - Friday</t>
+  </si>
+  <si>
+    <t>June 18 - Monday</t>
+  </si>
+  <si>
+    <t>June 19 - Tuesday</t>
+  </si>
+  <si>
+    <t>June 20 - Wedensday</t>
+  </si>
+  <si>
+    <t>June 21 - Thursday</t>
+  </si>
+  <si>
+    <t>June 22 - Friday</t>
+  </si>
+  <si>
+    <t>June 25 - Monday</t>
+  </si>
+  <si>
+    <t>June 26 - Tuesday</t>
+  </si>
+  <si>
+    <t>June 27 - Wedensday</t>
+  </si>
+  <si>
+    <t>June 28 - Thursday</t>
+  </si>
+  <si>
+    <t>June 29 - Friday</t>
+  </si>
+  <si>
+    <t>July 2 - Monday</t>
+  </si>
+  <si>
+    <t>July 3 - Tuesday</t>
+  </si>
+  <si>
+    <t>July 4 - Wednesday</t>
+  </si>
+  <si>
+    <t>July 5 - Thursday</t>
+  </si>
+  <si>
+    <t>July 6 - Friday</t>
+  </si>
+  <si>
+    <t>July 9 - Monday</t>
+  </si>
+  <si>
+    <t>July 10 - Tuesday</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Installment</t>
+  </si>
+  <si>
+    <t>Terminal commands</t>
+  </si>
+  <si>
+    <t>html/css</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>mobile responsiveness</t>
+  </si>
+  <si>
+    <t>normalize.css</t>
+  </si>
+  <si>
+    <t>media queries</t>
+  </si>
+  <si>
+    <t>gird</t>
+  </si>
+  <si>
+    <t>animation/keyframes</t>
+  </si>
+  <si>
+    <t>git/github</t>
+  </si>
+  <si>
+    <t>brnaches</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Final group - presentation</t>
+  </si>
+  <si>
+    <t>Final Group</t>
+  </si>
+  <si>
+    <t>Shipped Presentation</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>Object Oriented JavaScript Mini Challenges</t>
+  </si>
+  <si>
+    <t>Businesss Website</t>
+  </si>
+  <si>
+    <t>Micro-blog</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Rails</t>
+  </si>
+  <si>
+    <t>Sessions</t>
+  </si>
+  <si>
+    <t>Relational DB</t>
+  </si>
+  <si>
+    <t>API example</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,8 +702,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +777,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -467,7 +793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -512,8 +838,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -532,8 +879,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +927,27 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -908,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1467,4 +1843,633 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A3" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A10" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="17" customFormat="1" ht="20">
+      <c r="A19" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="B20" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="24" customHeight="1">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" s="17" customFormat="1" ht="20">
+      <c r="A24" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="17" customFormat="1" ht="20">
+      <c r="A31" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A36" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A41" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="16"/>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>206</v>
+      </c>
+      <c r="E42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" s="16"/>
+      <c r="D43" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45" s="16"/>
+      <c r="F45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A46" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="D48" t="s">
+        <v>210</v>
+      </c>
+      <c r="E48" t="s">
+        <v>210</v>
+      </c>
+      <c r="F48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A54" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A60" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A64" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="B66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" t="s">
+        <v>185</v>
+      </c>
+      <c r="F66" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="A69" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="D70" s="4"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" t="s">
+        <v>185</v>
+      </c>
+      <c r="F71" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" s="17" customFormat="1" ht="20">
+      <c r="B74" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" tooltip="c. Object Oriented JavaScript Mini Challenges"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
coding challnege on its way
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="309">
   <si>
     <t>January 16 Tuesday</t>
   </si>
@@ -933,6 +933,21 @@
   </si>
   <si>
     <t>DOM manipulation</t>
+  </si>
+  <si>
+    <t>Constructor Function</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Homewors Mindler</t>
+  </si>
+  <si>
+    <t>presentation of Mindler</t>
+  </si>
+  <si>
+    <t>end of JS???</t>
   </si>
 </sst>
 </file>
@@ -2821,7 +2836,6 @@
     <hyperlink ref="B20" r:id="rId1" tooltip="c. Object Oriented JavaScript Mini Challenges"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2834,16 +2848,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
@@ -3028,6 +3042,17 @@
         <v>232</v>
       </c>
     </row>
+    <row r="21" spans="1:6">
+      <c r="D21" t="s">
+        <v>304</v>
+      </c>
+      <c r="E21" t="s">
+        <v>305</v>
+      </c>
+      <c r="F21" t="s">
+        <v>306</v>
+      </c>
+    </row>
     <row r="26" spans="1:6" ht="20">
       <c r="A26" s="17" t="s">
         <v>196</v>
@@ -3065,6 +3090,11 @@
         <v>237</v>
       </c>
     </row>
+    <row r="28" spans="1:6">
+      <c r="B28" t="s">
+        <v>307</v>
+      </c>
+    </row>
     <row r="33" spans="1:6" ht="20">
       <c r="A33" s="17" t="s">
         <v>197</v>
@@ -3137,6 +3167,11 @@
       </c>
       <c r="F39" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="D40" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20">
@@ -3554,7 +3589,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>